<commit_message>
Added batching of files
</commit_message>
<xml_diff>
--- a/src/data/FounderImageURL60.xlsx
+++ b/src/data/FounderImageURL60.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin\OneDrive\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Data\Development\Flask\SurveyTool\SurveyTool\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F17BABE-9C8C-4F4C-8504-568CA5FA82FB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6130045F-2FC4-4E40-9CB9-E75B760437F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10815" xr2:uid="{2F6E9258-C4F4-4C68-AC54-21062944BF08}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{2F6E9258-C4F4-4C68-AC54-21062944BF08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="299">
   <si>
     <t>founder_identifier_uuid</t>
   </si>
@@ -532,24 +532,406 @@
   </si>
   <si>
     <t>https://images.crunchbase.com/image/upload/ptkjzpcrlz0strjm3en2.png</t>
+  </si>
+  <si>
+    <t>04174d4e-cd5e-1bd6-83c7-26ceb86c1c03</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1398470201/h7k3ii7udnxgmeleu8fw.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/h7k3ii7udnxgmeleu8fw.jpg</t>
+  </si>
+  <si>
+    <t>04aca15f-c662-c56d-7d7d-5939d4b79571</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1476767769/pyctluufcnnyrjvp7vlj.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/pyctluufcnnyrjvp7vlj.png</t>
+  </si>
+  <si>
+    <t>04cf766e-8cbf-4b92-0bcc-37ea24f60f4c</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1481330585/pcc9i4mtgqqh8o0lt8cr.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/pcc9i4mtgqqh8o0lt8cr.jpg</t>
+  </si>
+  <si>
+    <t>05068e05-77a6-76f8-fcd4-2741dd829822</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1471165839/angr1bibdegeczel4all.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/angr1bibdegeczel4all.png</t>
+  </si>
+  <si>
+    <t>0510dc0a-3bb4-2d16-a131-c29318a0ae01</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1453783334/wtuy38zcag9c2dwugbo5.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/wtuy38zcag9c2dwugbo5.png</t>
+  </si>
+  <si>
+    <t>05331482-d3ac-ea9d-53d5-0035f882ca19</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1452898145/fvqlmlxdnncvfk88dax2.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/fvqlmlxdnncvfk88dax2.png</t>
+  </si>
+  <si>
+    <t>053bbf43-71ef-4c25-05e1-69df8c011cc7</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1414528277/ctkil9m4b9zicb4qmywu.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ctkil9m4b9zicb4qmywu.jpg</t>
+  </si>
+  <si>
+    <t>0547cd9f-dd49-1f29-131e-05b8bd1c940c</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1421694888/vojp5wcum2whgsl8yjwv.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/vojp5wcum2whgsl8yjwv.jpg</t>
+  </si>
+  <si>
+    <t>054eb693-9c86-f121-4c71-fd9656440a41</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/t_cb-default-original/v1457132181/lj3j2dgazglpj8bgumjm.jpg</t>
+  </si>
+  <si>
+    <t>058df24f-6436-fc9f-18a3-d7718850abc4</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/t_cb-default-original/v1417424935/wxgwmwwidofoghxerryw.png</t>
+  </si>
+  <si>
+    <t>0597a759-cb95-fb9a-3ccc-7f542d0ef4eb</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1466154185/ha53dckdqfu0te8uxnkt.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ha53dckdqfu0te8uxnkt.jpg</t>
+  </si>
+  <si>
+    <t>05b0036e-4c5d-10f2-2c54-e44346b871e0</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1455596503/fvgxridsanozkdanwl7b.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/fvgxridsanozkdanwl7b.jpg</t>
+  </si>
+  <si>
+    <t>05b92eb8-a78a-4214-9abd-931279dc361e</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/ce6ahwgbp24axifqbri7</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ce6ahwgbp24axifqbri7</t>
+  </si>
+  <si>
+    <t>05c644be-c4c4-7611-5f95-2ef3f9de6f7f</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/kxw6blixqkuadn19mzbe</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/kxw6blixqkuadn19mzbe</t>
+  </si>
+  <si>
+    <t>05df457f-e161-9256-46ea-171e5ce1d3b1</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/ktkpvj9cvw0fmitepacr</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ktkpvj9cvw0fmitepacr</t>
+  </si>
+  <si>
+    <t>05e8c515-2abc-2534-c63d-560cf5af1507</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/ev1guwmhmcrhqivgapkh</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ev1guwmhmcrhqivgapkh</t>
+  </si>
+  <si>
+    <t>05f6c2a3-4e7b-3ab7-def8-8dc1215d448b</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1414472112/evkvwyzr7xiafured6vw.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/evkvwyzr7xiafured6vw.jpg</t>
+  </si>
+  <si>
+    <t>060048a6-4665-8d93-4684-adb2e198315c</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1400823455/h0plan8jow6l0vjndftl.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/h0plan8jow6l0vjndftl.jpg</t>
+  </si>
+  <si>
+    <t>06078528-0306-79e4-e1a1-de01ccaf66c5</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1456645752/o8tsojvgyydehowl04wb.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/o8tsojvgyydehowl04wb.png</t>
+  </si>
+  <si>
+    <t>06086ba2-9273-7f5c-565d-0b545ad0d2bd</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/a9kjc7k0zfyogp1hyi0y</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/a9kjc7k0zfyogp1hyi0y</t>
+  </si>
+  <si>
+    <t>0617bb54-8a66-1325-03cb-c29804a5007d</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1427242630/levpyq6zydkm7nocrnkr.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/levpyq6zydkm7nocrnkr.png</t>
+  </si>
+  <si>
+    <t>061ae03f-1d4d-23fc-ac99-cd8db20f71ea</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1486270034/ny2wpoyfeyiekodrbjhs.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ny2wpoyfeyiekodrbjhs.jpg</t>
+  </si>
+  <si>
+    <t>06305a9f-0600-e8f3-a9cb-8b1648ff07b5</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1421721745/imojnebaefdpsc3obh2b.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/imojnebaefdpsc3obh2b.png</t>
+  </si>
+  <si>
+    <t>0649c5d0-533b-03e9-5b39-c21869b2a898</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1468939560/dpect1gvickdbqxeltcu.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/dpect1gvickdbqxeltcu.jpg</t>
+  </si>
+  <si>
+    <t>06913245-a0c1-e9ab-1e87-1e6999eae007</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1451531132/arkifjnirdyvbl7oq9nh.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/arkifjnirdyvbl7oq9nh.jpg</t>
+  </si>
+  <si>
+    <t>069e3a7c-5a9c-f30b-9858-9a4975e4aff8</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1474406794/npakfzwlkihfqx0vilhk.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/npakfzwlkihfqx0vilhk.png</t>
+  </si>
+  <si>
+    <t>06a60d30-2d0c-41d6-94be-a8b728cc94a1</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/fxdgrzs9m5qfrzswaibg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/fxdgrzs9m5qfrzswaibg</t>
+  </si>
+  <si>
+    <t>06ac2a33-9e7d-41b3-8ee6-b2f1d7dd6f79</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/ypggozk2sccouxuc8pvp</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ypggozk2sccouxuc8pvp</t>
+  </si>
+  <si>
+    <t>06ec420a-bcfc-bd47-a7bc-34ae4f82ec15</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1483956753/kfl521gb4tc2dmkeaizv.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/kfl521gb4tc2dmkeaizv.png</t>
+  </si>
+  <si>
+    <t>06fdc68c-5d1d-95f3-34a2-e3aba5e603d1</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1431683440/hta0s1b0xncguz8bf6xg.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/hta0s1b0xncguz8bf6xg.png</t>
+  </si>
+  <si>
+    <t>071ea137-1394-f72a-587e-b12aecf76b33</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1412093736/yf8yjtaixatsp4oeeagk.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/yf8yjtaixatsp4oeeagk.jpg</t>
+  </si>
+  <si>
+    <t>072adb34-05a9-4e72-9844-cccb2654d9d2</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/wb6ggyyh8kguzuqlumlz</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/wb6ggyyh8kguzuqlumlz</t>
+  </si>
+  <si>
+    <t>072fbf99-4c3b-ebd5-6021-45d2becf84d4</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/s89dkkepq1xrwvwriock</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/s89dkkepq1xrwvwriock</t>
+  </si>
+  <si>
+    <t>07532513-d6ba-a560-5af5-d0f705d8fbb2</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1505814456/egwluja8ytwa9gkbmmy7.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/egwluja8ytwa9gkbmmy7.png</t>
+  </si>
+  <si>
+    <t>07585a4e-497b-7497-8fef-ac465872f74f</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1431590399/pj88uvnnzytjwcsox3g3.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/pj88uvnnzytjwcsox3g3.jpg</t>
+  </si>
+  <si>
+    <t>075e679c-7a54-401f-ae27-04cd4c8c913c</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/rrq3lgtrxtvidyp6o8ou</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/rrq3lgtrxtvidyp6o8ou</t>
+  </si>
+  <si>
+    <t>07645c04-3628-4b7e-c8f2-960fb6a74e10</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1430484303/dvcpaq3kkntfreeapuuo.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/dvcpaq3kkntfreeapuuo.jpg</t>
+  </si>
+  <si>
+    <t>076bd0e1-799b-4f04-ade7-b1aae828eff3</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/vdqqnjbtvvroyw93varf</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/vdqqnjbtvvroyw93varf</t>
+  </si>
+  <si>
+    <t>077154ae-4c5c-cadf-211f-96ef272d0bd1</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/p07gfcw0jaolrkpc1bqi</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/p07gfcw0jaolrkpc1bqi</t>
+  </si>
+  <si>
+    <t>078b2c4d-2baf-a867-2a29-153f2e4a65aa</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1431269558/uorotv7qgfrdlgxbq838.jpg</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/uorotv7qgfrdlgxbq838.jpg</t>
+  </si>
+  <si>
+    <t>079207ab-f588-4a01-8e88-c918653c49c8</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/ac0jz9dj2kjiph5bnhxf</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/ac0jz9dj2kjiph5bnhxf</t>
+  </si>
+  <si>
+    <t>07a0340e-892e-9776-9efb-4c505bb1091e</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/v1492591867/av7tdlmziwxkmzm6qmo7.png</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/av7tdlmziwxkmzm6qmo7.png</t>
+  </si>
+  <si>
+    <t>07ad1d2d-21de-bf97-9e3d-9534d62c65c6</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/idxq1tigutw1myjijrwf</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/idxq1tigutw1myjijrwf</t>
+  </si>
+  <si>
+    <t>07bbed44-3e3b-b37c-1c52-7e9cd25e6204</t>
+  </si>
+  <si>
+    <t>https://res.cloudinary.com/crunchbase-production/image/upload/b7cksy7wajqaqeg37xyt</t>
+  </si>
+  <si>
+    <t>https://images.crunchbase.com/image/upload/b7cksy7wajqaqeg37xyt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -572,16 +954,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -894,15 +1274,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52A2DDB4-239A-4007-832E-E114607AD348}">
-  <dimension ref="A1:D60"/>
+  <dimension ref="A1:D101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD60"/>
+      <selection sqref="A1:D101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -913,7 +1293,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -923,11 +1303,11 @@
       <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -937,11 +1317,11 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -955,7 +1335,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -965,11 +1345,11 @@
       <c r="C5" t="s">
         <v>13</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -979,11 +1359,11 @@
       <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -997,7 +1377,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -1011,7 +1391,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -1025,7 +1405,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>10</v>
       </c>
@@ -1039,7 +1419,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1053,7 +1433,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>12</v>
       </c>
@@ -1067,7 +1447,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>13</v>
       </c>
@@ -1081,671 +1461,1239 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
+        <v>39</v>
+      </c>
+      <c r="C14" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>42</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>17</v>
+      </c>
+      <c r="B16" t="s">
+        <v>45</v>
+      </c>
+      <c r="C16" t="s">
+        <v>46</v>
+      </c>
+      <c r="D16" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>18</v>
+      </c>
+      <c r="B17" t="s">
+        <v>48</v>
+      </c>
+      <c r="C17" t="s">
+        <v>49</v>
+      </c>
+      <c r="D17" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>51</v>
+      </c>
+      <c r="C18" t="s">
+        <v>52</v>
+      </c>
+      <c r="D18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C19" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>21</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>22</v>
+      </c>
+      <c r="B21" t="s">
+        <v>60</v>
+      </c>
+      <c r="C21" t="s">
+        <v>61</v>
+      </c>
+      <c r="D21" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>24</v>
+      </c>
+      <c r="B22" t="s">
+        <v>63</v>
+      </c>
+      <c r="C22" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>25</v>
+      </c>
+      <c r="B23" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" t="s">
+        <v>67</v>
+      </c>
+      <c r="D23" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>27</v>
+      </c>
+      <c r="B24" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" t="s">
+        <v>70</v>
+      </c>
+      <c r="D24" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>73</v>
+      </c>
+      <c r="D25" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>29</v>
+      </c>
+      <c r="B26" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D26" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>30</v>
+      </c>
+      <c r="B27" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" t="s">
+        <v>79</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>31</v>
+      </c>
+      <c r="B28" t="s">
+        <v>81</v>
+      </c>
+      <c r="C28" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>32</v>
+      </c>
+      <c r="B29" t="s">
+        <v>84</v>
+      </c>
+      <c r="C29" t="s">
+        <v>85</v>
+      </c>
+      <c r="D29" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>33</v>
+      </c>
+      <c r="B30" t="s">
+        <v>87</v>
+      </c>
+      <c r="C30" t="s">
+        <v>88</v>
+      </c>
+      <c r="D30" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>34</v>
+      </c>
+      <c r="B31" t="s">
+        <v>90</v>
+      </c>
+      <c r="C31" t="s">
+        <v>91</v>
+      </c>
+      <c r="D31" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>35</v>
+      </c>
+      <c r="B32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C32" t="s">
+        <v>94</v>
+      </c>
+      <c r="D32" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
         <v>36</v>
       </c>
-      <c r="C14" t="s">
+      <c r="B33" t="s">
+        <v>96</v>
+      </c>
+      <c r="C33" t="s">
+        <v>97</v>
+      </c>
+      <c r="D33" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
         <v>37</v>
       </c>
-      <c r="D14" t="s">
+      <c r="B34" t="s">
+        <v>99</v>
+      </c>
+      <c r="C34" t="s">
+        <v>100</v>
+      </c>
+      <c r="D34" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A35">
         <v>38</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>15</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="B35" t="s">
+        <v>102</v>
+      </c>
+      <c r="C35" t="s">
+        <v>103</v>
+      </c>
+      <c r="D35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A36">
         <v>39</v>
       </c>
-      <c r="C15" t="s">
+      <c r="B36" t="s">
+        <v>105</v>
+      </c>
+      <c r="C36" t="s">
+        <v>106</v>
+      </c>
+      <c r="D36" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37">
         <v>40</v>
       </c>
-      <c r="D15" t="s">
+      <c r="B37" t="s">
+        <v>107</v>
+      </c>
+      <c r="C37" t="s">
+        <v>108</v>
+      </c>
+      <c r="D37" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38">
         <v>41</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>16</v>
-      </c>
-      <c r="B16" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" t="s">
+      <c r="B38" t="s">
+        <v>110</v>
+      </c>
+      <c r="C38" t="s">
+        <v>111</v>
+      </c>
+      <c r="D38" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39">
         <v>43</v>
       </c>
-      <c r="D16" t="s">
+      <c r="B39" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" t="s">
+        <v>114</v>
+      </c>
+      <c r="D39" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40">
         <v>44</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>17</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B40" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41">
         <v>45</v>
       </c>
-      <c r="C17" t="s">
+      <c r="B41" t="s">
+        <v>118</v>
+      </c>
+      <c r="C41" t="s">
+        <v>119</v>
+      </c>
+      <c r="D41" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42">
         <v>46</v>
       </c>
-      <c r="D17" t="s">
+      <c r="B42" t="s">
+        <v>121</v>
+      </c>
+      <c r="C42" t="s">
+        <v>122</v>
+      </c>
+      <c r="D42" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
         <v>47</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>18</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="B43" t="s">
+        <v>124</v>
+      </c>
+      <c r="C43" t="s">
+        <v>125</v>
+      </c>
+      <c r="D43" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
         <v>48</v>
       </c>
-      <c r="C18" t="s">
+      <c r="B44" t="s">
+        <v>127</v>
+      </c>
+      <c r="C44" t="s">
+        <v>128</v>
+      </c>
+      <c r="D44" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
         <v>49</v>
       </c>
-      <c r="D18" t="s">
+      <c r="B45" t="s">
+        <v>130</v>
+      </c>
+      <c r="C45" t="s">
+        <v>131</v>
+      </c>
+      <c r="D45" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
         <v>50</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>19</v>
-      </c>
-      <c r="B19" t="s">
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="C46" t="s">
+        <v>134</v>
+      </c>
+      <c r="D46" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A47">
         <v>51</v>
       </c>
-      <c r="C19" t="s">
+      <c r="B47" t="s">
+        <v>136</v>
+      </c>
+      <c r="C47" t="s">
+        <v>137</v>
+      </c>
+      <c r="D47" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A48">
         <v>52</v>
       </c>
-      <c r="D19" t="s">
+      <c r="B48" t="s">
+        <v>139</v>
+      </c>
+      <c r="C48" t="s">
+        <v>140</v>
+      </c>
+      <c r="D48" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>20</v>
-      </c>
-      <c r="B20" t="s">
+      <c r="B49" t="s">
+        <v>142</v>
+      </c>
+      <c r="C49" t="s">
+        <v>143</v>
+      </c>
+      <c r="D49" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50">
         <v>54</v>
       </c>
-      <c r="C20" t="s">
+      <c r="B50" t="s">
+        <v>145</v>
+      </c>
+      <c r="C50" t="s">
+        <v>146</v>
+      </c>
+      <c r="D50" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A51">
         <v>55</v>
       </c>
-      <c r="D20" t="s">
+      <c r="B51" t="s">
+        <v>148</v>
+      </c>
+      <c r="C51" t="s">
+        <v>149</v>
+      </c>
+      <c r="D51" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
         <v>56</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>21</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B52" t="s">
+        <v>151</v>
+      </c>
+      <c r="C52" t="s">
+        <v>152</v>
+      </c>
+      <c r="D52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53">
         <v>57</v>
       </c>
-      <c r="C21" t="s">
+      <c r="B53" t="s">
+        <v>154</v>
+      </c>
+      <c r="C53" t="s">
+        <v>155</v>
+      </c>
+      <c r="D53" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
         <v>58</v>
       </c>
-      <c r="D21" t="s">
+      <c r="B54" t="s">
+        <v>157</v>
+      </c>
+      <c r="C54" t="s">
+        <v>158</v>
+      </c>
+      <c r="D54" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55">
         <v>59</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>22</v>
-      </c>
-      <c r="B22" t="s">
+      <c r="B55" t="s">
+        <v>160</v>
+      </c>
+      <c r="C55" t="s">
+        <v>161</v>
+      </c>
+      <c r="D55" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
         <v>60</v>
       </c>
-      <c r="C22" t="s">
+      <c r="B56" t="s">
+        <v>163</v>
+      </c>
+      <c r="C56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D56" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
         <v>61</v>
       </c>
-      <c r="D22" t="s">
+      <c r="B57" t="s">
+        <v>166</v>
+      </c>
+      <c r="C57" t="s">
+        <v>167</v>
+      </c>
+      <c r="D57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
         <v>62</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>24</v>
-      </c>
-      <c r="B23" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B58" t="s">
+        <v>169</v>
+      </c>
+      <c r="C58" t="s">
+        <v>170</v>
+      </c>
+      <c r="D58" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
         <v>64</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B59" t="s">
+        <v>172</v>
+      </c>
+      <c r="C59" t="s">
+        <v>173</v>
+      </c>
+      <c r="D59" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
         <v>65</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>25</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="B60" t="s">
+        <v>175</v>
+      </c>
+      <c r="C60" t="s">
+        <v>176</v>
+      </c>
+      <c r="D60" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
         <v>66</v>
       </c>
-      <c r="C24" t="s">
+      <c r="B61" t="s">
+        <v>178</v>
+      </c>
+      <c r="C61" t="s">
+        <v>179</v>
+      </c>
+      <c r="D61" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
         <v>67</v>
       </c>
-      <c r="D24" t="s">
+      <c r="B62" t="s">
+        <v>181</v>
+      </c>
+      <c r="C62" t="s">
+        <v>182</v>
+      </c>
+      <c r="D62" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
         <v>68</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25">
-        <v>26</v>
-      </c>
-      <c r="B25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C25" t="s">
-        <v>67</v>
-      </c>
-      <c r="D25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26">
-        <v>27</v>
-      </c>
-      <c r="B26" t="s">
+      <c r="B63" t="s">
+        <v>184</v>
+      </c>
+      <c r="C63" t="s">
+        <v>185</v>
+      </c>
+      <c r="D63" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
         <v>69</v>
       </c>
-      <c r="C26" t="s">
+      <c r="B64" t="s">
+        <v>187</v>
+      </c>
+      <c r="C64" t="s">
+        <v>188</v>
+      </c>
+      <c r="D64" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A65">
         <v>70</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B65" t="s">
+        <v>190</v>
+      </c>
+      <c r="C65" t="s">
+        <v>191</v>
+      </c>
+      <c r="D65" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
         <v>71</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27">
-        <v>28</v>
-      </c>
-      <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" t="s">
+      <c r="B66" t="s">
+        <v>193</v>
+      </c>
+      <c r="C66" t="s">
+        <v>194</v>
+      </c>
+      <c r="D66" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
         <v>73</v>
       </c>
-      <c r="D27" t="s">
+      <c r="B67" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" t="s">
+        <v>196</v>
+      </c>
+      <c r="D67" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
         <v>74</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28">
-        <v>29</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="B68" t="s">
+        <v>197</v>
+      </c>
+      <c r="C68" t="s">
+        <v>198</v>
+      </c>
+      <c r="D68" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
         <v>75</v>
       </c>
-      <c r="C28" t="s">
+      <c r="B69" t="s">
+        <v>200</v>
+      </c>
+      <c r="C69" t="s">
+        <v>201</v>
+      </c>
+      <c r="D69" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
         <v>76</v>
       </c>
-      <c r="D28" t="s">
+      <c r="B70" t="s">
+        <v>203</v>
+      </c>
+      <c r="C70" t="s">
+        <v>204</v>
+      </c>
+      <c r="D70" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
         <v>77</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29">
-        <v>30</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="B71" t="s">
+        <v>206</v>
+      </c>
+      <c r="C71" t="s">
+        <v>207</v>
+      </c>
+      <c r="D71" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
         <v>78</v>
       </c>
-      <c r="C29" t="s">
+      <c r="B72" t="s">
+        <v>209</v>
+      </c>
+      <c r="C72" t="s">
+        <v>210</v>
+      </c>
+      <c r="D72" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
         <v>79</v>
       </c>
-      <c r="D29" t="s">
+      <c r="B73" t="s">
+        <v>212</v>
+      </c>
+      <c r="C73" t="s">
+        <v>213</v>
+      </c>
+      <c r="D73" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
         <v>80</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30">
-        <v>31</v>
-      </c>
-      <c r="B30" t="s">
+      <c r="B74" t="s">
+        <v>215</v>
+      </c>
+      <c r="C74" t="s">
+        <v>216</v>
+      </c>
+      <c r="D74" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
         <v>81</v>
       </c>
-      <c r="C30" t="s">
+      <c r="B75" t="s">
+        <v>218</v>
+      </c>
+      <c r="C75" t="s">
+        <v>219</v>
+      </c>
+      <c r="D75" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76">
         <v>82</v>
       </c>
-      <c r="D30" t="s">
+      <c r="B76" t="s">
+        <v>221</v>
+      </c>
+      <c r="C76" t="s">
+        <v>222</v>
+      </c>
+      <c r="D76" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77">
         <v>83</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31">
-        <v>32</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="B77" t="s">
+        <v>224</v>
+      </c>
+      <c r="C77" t="s">
+        <v>225</v>
+      </c>
+      <c r="D77" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78">
         <v>84</v>
       </c>
-      <c r="C31" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="B78" t="s">
+        <v>227</v>
+      </c>
+      <c r="C78" t="s">
+        <v>228</v>
+      </c>
+      <c r="D78" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
         <v>86</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32">
-        <v>33</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="B79" t="s">
+        <v>230</v>
+      </c>
+      <c r="C79" t="s">
+        <v>231</v>
+      </c>
+      <c r="D79" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
         <v>87</v>
       </c>
-      <c r="C32" t="s">
+      <c r="B80" t="s">
+        <v>233</v>
+      </c>
+      <c r="C80" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A81">
         <v>88</v>
       </c>
-      <c r="D32" t="s">
+      <c r="B81" t="s">
+        <v>236</v>
+      </c>
+      <c r="C81" t="s">
+        <v>237</v>
+      </c>
+      <c r="D81" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A82">
         <v>89</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33">
-        <v>34</v>
-      </c>
-      <c r="B33" t="s">
-        <v>90</v>
-      </c>
-      <c r="C33" t="s">
+      <c r="B82" t="s">
+        <v>239</v>
+      </c>
+      <c r="C82" t="s">
+        <v>240</v>
+      </c>
+      <c r="D82" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A83">
         <v>91</v>
       </c>
-      <c r="D33" t="s">
+      <c r="B83" t="s">
+        <v>242</v>
+      </c>
+      <c r="C83" t="s">
+        <v>243</v>
+      </c>
+      <c r="D83" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A84">
         <v>92</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34">
-        <v>35</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="B84" t="s">
+        <v>245</v>
+      </c>
+      <c r="C84" t="s">
+        <v>246</v>
+      </c>
+      <c r="D84" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A85">
         <v>93</v>
       </c>
-      <c r="C34" t="s">
-        <v>94</v>
-      </c>
-      <c r="D34" t="s">
+      <c r="B85" t="s">
+        <v>248</v>
+      </c>
+      <c r="C85" t="s">
+        <v>249</v>
+      </c>
+      <c r="D85" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A86">
         <v>95</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35">
-        <v>36</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="B86" t="s">
+        <v>251</v>
+      </c>
+      <c r="C86" t="s">
+        <v>252</v>
+      </c>
+      <c r="D86" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A87">
         <v>96</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B87" t="s">
+        <v>254</v>
+      </c>
+      <c r="C87" t="s">
+        <v>255</v>
+      </c>
+      <c r="D87" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A88">
         <v>97</v>
       </c>
-      <c r="D35" t="s">
+      <c r="B88" t="s">
+        <v>257</v>
+      </c>
+      <c r="C88" t="s">
+        <v>258</v>
+      </c>
+      <c r="D88" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A89">
         <v>98</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36">
-        <v>37</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="B89" t="s">
+        <v>260</v>
+      </c>
+      <c r="C89" t="s">
+        <v>261</v>
+      </c>
+      <c r="D89" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A90">
         <v>99</v>
       </c>
-      <c r="C36" t="s">
+      <c r="B90" t="s">
+        <v>263</v>
+      </c>
+      <c r="C90" t="s">
+        <v>264</v>
+      </c>
+      <c r="D90" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A91">
         <v>100</v>
       </c>
-      <c r="D36" t="s">
+      <c r="B91" t="s">
+        <v>266</v>
+      </c>
+      <c r="C91" t="s">
+        <v>267</v>
+      </c>
+      <c r="D91" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A92">
         <v>101</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37">
-        <v>38</v>
-      </c>
-      <c r="B37" t="s">
+      <c r="B92" t="s">
+        <v>269</v>
+      </c>
+      <c r="C92" t="s">
+        <v>270</v>
+      </c>
+      <c r="D92" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A93">
         <v>102</v>
       </c>
-      <c r="C37" t="s">
+      <c r="B93" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C93" t="s">
+        <v>273</v>
+      </c>
+      <c r="D93" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A94">
         <v>103</v>
       </c>
-      <c r="D37" t="s">
+      <c r="B94" t="s">
+        <v>275</v>
+      </c>
+      <c r="C94" t="s">
+        <v>276</v>
+      </c>
+      <c r="D94" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A95">
         <v>104</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38">
-        <v>39</v>
-      </c>
-      <c r="B38" t="s">
+      <c r="B95" t="s">
+        <v>278</v>
+      </c>
+      <c r="C95" t="s">
+        <v>279</v>
+      </c>
+      <c r="D95" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A96">
         <v>105</v>
       </c>
-      <c r="C38" t="s">
+      <c r="B96" t="s">
+        <v>281</v>
+      </c>
+      <c r="C96" t="s">
+        <v>282</v>
+      </c>
+      <c r="D96" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A97">
         <v>106</v>
       </c>
-      <c r="D38" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39">
-        <v>40</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="B97" t="s">
+        <v>284</v>
+      </c>
+      <c r="C97" t="s">
+        <v>285</v>
+      </c>
+      <c r="D97" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A98">
         <v>107</v>
       </c>
-      <c r="C39" t="s">
+      <c r="B98" t="s">
+        <v>287</v>
+      </c>
+      <c r="C98" t="s">
+        <v>288</v>
+      </c>
+      <c r="D98" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A99">
         <v>108</v>
       </c>
-      <c r="D39" t="s">
+      <c r="B99" t="s">
+        <v>290</v>
+      </c>
+      <c r="C99" t="s">
+        <v>291</v>
+      </c>
+      <c r="D99" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A100">
         <v>109</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40">
-        <v>41</v>
-      </c>
-      <c r="B40" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="B100" t="s">
+        <v>293</v>
+      </c>
+      <c r="C100" t="s">
+        <v>294</v>
+      </c>
+      <c r="D100" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A101">
         <v>111</v>
       </c>
-      <c r="D40" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41">
-        <v>42</v>
-      </c>
-      <c r="B41" t="s">
-        <v>110</v>
-      </c>
-      <c r="C41" t="s">
-        <v>111</v>
-      </c>
-      <c r="D41" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42">
-        <v>43</v>
-      </c>
-      <c r="B42" t="s">
-        <v>113</v>
-      </c>
-      <c r="C42" t="s">
-        <v>114</v>
-      </c>
-      <c r="D42" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43">
-        <v>44</v>
-      </c>
-      <c r="B43" t="s">
-        <v>115</v>
-      </c>
-      <c r="C43" t="s">
-        <v>116</v>
-      </c>
-      <c r="D43" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44">
-        <v>45</v>
-      </c>
-      <c r="B44" t="s">
-        <v>118</v>
-      </c>
-      <c r="C44" t="s">
-        <v>119</v>
-      </c>
-      <c r="D44" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45">
-        <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>121</v>
-      </c>
-      <c r="C45" t="s">
-        <v>122</v>
-      </c>
-      <c r="D45" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46">
-        <v>47</v>
-      </c>
-      <c r="B46" t="s">
-        <v>124</v>
-      </c>
-      <c r="C46" t="s">
-        <v>125</v>
-      </c>
-      <c r="D46" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47">
-        <v>48</v>
-      </c>
-      <c r="B47" t="s">
-        <v>127</v>
-      </c>
-      <c r="C47" t="s">
-        <v>128</v>
-      </c>
-      <c r="D47" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48">
-        <v>49</v>
-      </c>
-      <c r="B48" t="s">
-        <v>130</v>
-      </c>
-      <c r="C48" t="s">
-        <v>131</v>
-      </c>
-      <c r="D48" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49">
-        <v>50</v>
-      </c>
-      <c r="B49" t="s">
-        <v>133</v>
-      </c>
-      <c r="C49" t="s">
-        <v>134</v>
-      </c>
-      <c r="D49" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50">
-        <v>51</v>
-      </c>
-      <c r="B50" t="s">
-        <v>136</v>
-      </c>
-      <c r="C50" t="s">
-        <v>137</v>
-      </c>
-      <c r="D50" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51">
-        <v>52</v>
-      </c>
-      <c r="B51" t="s">
-        <v>139</v>
-      </c>
-      <c r="C51" t="s">
-        <v>140</v>
-      </c>
-      <c r="D51" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52">
-        <v>53</v>
-      </c>
-      <c r="B52" t="s">
-        <v>142</v>
-      </c>
-      <c r="C52" t="s">
-        <v>143</v>
-      </c>
-      <c r="D52" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53">
-        <v>54</v>
-      </c>
-      <c r="B53" t="s">
-        <v>145</v>
-      </c>
-      <c r="C53" t="s">
-        <v>146</v>
-      </c>
-      <c r="D53" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54">
-        <v>55</v>
-      </c>
-      <c r="B54" t="s">
-        <v>148</v>
-      </c>
-      <c r="C54" t="s">
-        <v>149</v>
-      </c>
-      <c r="D54" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>56</v>
-      </c>
-      <c r="B55" t="s">
-        <v>151</v>
-      </c>
-      <c r="C55" t="s">
-        <v>152</v>
-      </c>
-      <c r="D55" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>57</v>
-      </c>
-      <c r="B56" t="s">
-        <v>154</v>
-      </c>
-      <c r="C56" t="s">
-        <v>155</v>
-      </c>
-      <c r="D56" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>58</v>
-      </c>
-      <c r="B57" t="s">
-        <v>157</v>
-      </c>
-      <c r="C57" t="s">
-        <v>158</v>
-      </c>
-      <c r="D57" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>59</v>
-      </c>
-      <c r="B58" t="s">
-        <v>160</v>
-      </c>
-      <c r="C58" t="s">
-        <v>161</v>
-      </c>
-      <c r="D58" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>60</v>
-      </c>
-      <c r="B59" t="s">
-        <v>163</v>
-      </c>
-      <c r="C59" t="s">
-        <v>164</v>
-      </c>
-      <c r="D59" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>61</v>
-      </c>
-      <c r="B60" t="s">
-        <v>166</v>
-      </c>
-      <c r="C60" t="s">
-        <v>167</v>
-      </c>
-      <c r="D60" t="s">
-        <v>168</v>
+      <c r="B101" t="s">
+        <v>296</v>
+      </c>
+      <c r="C101" t="s">
+        <v>297</v>
+      </c>
+      <c r="D101" t="s">
+        <v>298</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{C7BA55B0-0E34-4201-9925-41AF3DC5BF6B}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{05A4AF7C-63B2-4420-8D26-DC6EDBBFB2F5}"/>
-    <hyperlink ref="D3" r:id="rId3" xr:uid="{1F8B644C-5E28-490E-B74D-14213F8BEFBD}"/>
-    <hyperlink ref="D5" r:id="rId4" xr:uid="{43C00AFF-1A3B-48A0-A279-E1A31BE4031C}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>